<commit_message>
current field in securities and import
</commit_message>
<xml_diff>
--- a/lib/tasks/IW_MISSING.xlsx
+++ b/lib/tasks/IW_MISSING.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>FUND</t>
   </si>
@@ -30,9 +30,6 @@
     <t>Ironworkers Local 11 Benefit Funds</t>
   </si>
   <si>
-    <t>Iron Workers Local 201 Washington DC</t>
-  </si>
-  <si>
     <t>Ironworkers Local 3 Pittsburgh</t>
   </si>
   <si>
@@ -57,25 +54,53 @@
     <t>BNY</t>
   </si>
   <si>
-    <t>Asked MB to get it set up through Dave Corrado</t>
+    <t>Call Jessica Schneider</t>
+  </si>
+  <si>
+    <t>Should be on BNY</t>
+  </si>
+  <si>
+    <t>Regions Bank</t>
+  </si>
+  <si>
+    <t>Call Admin back</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="13"/>
       <color rgb="FF555555"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -95,14 +120,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -432,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -449,10 +486,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16">
@@ -460,10 +497,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16">
@@ -471,34 +508,42 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="16">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" spans="1:3" ht="16">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="16">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="16">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
+      <c r="B6" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>